<commit_message>
Working on laser jobs statistics
</commit_message>
<xml_diff>
--- a/persistence/data/laserJobs.xlsx
+++ b/persistence/data/laserJobs.xlsx
@@ -9,14 +9,14 @@
     <sheet name="LaserJobs" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -25,6 +25,11 @@
     <font>
       <name val="Arial"/>
       <charset val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -48,9 +53,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,13 +332,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <cols>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="19.7109375" customWidth="1" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" min="14" max="14"/>
+    <col width="14.140625" customWidth="1" min="15" max="15"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -355,9 +367,9 @@
           <t>Material</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Cut_Raster</t>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>JobType</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -375,9 +387,9 @@
           <t>DPI</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Freq</t>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -385,12 +397,32 @@
           <t>Passes</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>RasterDepth</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Depth</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>VectorSorting</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>FrequencyAutomatic</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>EngraveDirection</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>ImageDithering</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Others</t>
         </is>
@@ -400,24 +432,14 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>pmma</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Vector</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -442,15 +464,21 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1/0</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>-1</v>
       </c>
       <c r="L2" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -460,24 +488,14 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>pmma</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Raster</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -495,14 +513,12 @@
           <t>900</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
+      <c r="I3" t="n">
+        <v>-1</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -511,6 +527,21 @@
         </is>
       </c>
       <c r="L3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -520,24 +551,14 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>pmma</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -562,7 +583,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -571,6 +592,24 @@
         </is>
       </c>
       <c r="L4" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -580,24 +619,14 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>pmma</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -622,7 +651,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -631,6 +660,24 @@
         </is>
       </c>
       <c r="L5" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -640,24 +687,14 @@
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>david</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>pmma</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Raster</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -675,14 +712,12 @@
           <t>900</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
+      <c r="I6" t="n">
+        <v>-1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -691,6 +726,21 @@
         </is>
       </c>
       <c r="L6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -702,12 +752,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>sansanda</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -717,7 +767,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Vector</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -742,15 +792,21 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1/0</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>-1</v>
       </c>
       <c r="L7" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -762,22 +818,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>sansanda</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>pmma2</t>
+          <t>pmma</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Raster</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -795,14 +851,12 @@
           <t>900</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
+      <c r="I8" t="n">
+        <v>-1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -811,6 +865,21 @@
         </is>
       </c>
       <c r="L8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -822,22 +891,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>david2</t>
+          <t>sansanda</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>pmma2</t>
+          <t>pmma</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -862,7 +931,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1/0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -871,6 +940,24 @@
         </is>
       </c>
       <c r="L9" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Top-Down</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>
@@ -882,22 +969,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>sansanda</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2020-01-07</t>
+          <t>2020-01-08</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>pmma</t>
+          <t>pmma6</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Cut</t>
+          <t>Vector</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -922,15 +1009,79 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1/0</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>-1</v>
       </c>
       <c r="L10" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2020-01-08</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Vector</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>

</xml_diff>